<commit_message>
added site url to excel sheet
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsa\Practice_Selenium\TestAutomationEcommerceSite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D5FE5A8-7B7A-452E-A01D-CCB4ADD7CE27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ED0E97-DBB3-4055-908F-E58EF5EB47FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{03A41125-3342-46AB-A804-674B77AA42A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>samsal81@usa.com</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -408,7 +415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9A2468-F0FA-4325-9BDE-6715FD991D42}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -438,4 +447,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177DE8F-9961-4AE3-9C3A-7230ED34224B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>